<commit_message>
Check Model Type: Ensure that the loaded model is of the correct type (e.g., a scikit-learn model) and that it has a predict method. For example, if you have used scikit-learn for model training, it should have the predict method.
</commit_message>
<xml_diff>
--- a/Datasets/Cleaned Data.xlsx
+++ b/Datasets/Cleaned Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Educational\Projects\Parkinsons Disease Prediction\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664C2B93-4489-41F5-BAAC-14D1D7F2B0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB14FD-80A2-4818-9C61-67B1FFE60FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,11 +453,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>